<commit_message>
testing and added block detection decisions
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4041CFB6-8B8A-4744-9124-A8F1B5A78BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{4041CFB6-8B8A-4744-9124-A8F1B5A78BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5E05D61-0122-0C47-85F4-0528842FC30D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26440" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25240" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>The Display Week in cell E4  represents the starting week to display in the project schedule in cell I4. The project start date is considered Week 1. To change the display week, simply enter a new week number in cell E4.
 The starting date for each week, starting with the display week from cell E4, starts in cell I4 and is auto calculated. There are 8 weeks represented in this view from cell I4 through cell BF4.
@@ -1288,6 +1288,10 @@
     <xf numFmtId="168" fontId="10" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="169" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1297,10 +1301,6 @@
     <xf numFmtId="169" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20% - Accent1" xfId="31" builtinId="30" customBuiltin="1"/>
@@ -1358,67 +1358,7 @@
     <cellStyle name="Warning Text" xfId="26" builtinId="11" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill>
@@ -1575,15 +1515,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="totalRow" dxfId="18"/>
-      <tableStyleElement type="firstColumn" dxfId="17"/>
-      <tableStyleElement type="lastColumn" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="15"/>
-      <tableStyleElement type="secondRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="12"/>
+      <tableStyleElement type="wholeTable" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="totalRow" dxfId="12"/>
+      <tableStyleElement type="firstColumn" dxfId="11"/>
+      <tableStyleElement type="lastColumn" dxfId="10"/>
+      <tableStyleElement type="firstRowStripe" dxfId="9"/>
+      <tableStyleElement type="secondRowStripe" dxfId="8"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="7"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2002,7 +1942,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V12" sqref="V12"/>
+      <selection pane="bottomLeft" activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2028,58 +1968,61 @@
       <c r="C1" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="83">
+      <c r="E1" s="81">
         <f ca="1">TODAY()</f>
         <v>44868</v>
       </c>
-      <c r="F1" s="83"/>
-      <c r="H1" s="80">
+      <c r="F1" s="81"/>
+      <c r="H1" s="82">
         <f ca="1">H2</f>
         <v>44868</v>
       </c>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="80">
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="82">
         <f ca="1">O2</f>
         <v>44875</v>
       </c>
-      <c r="P1" s="81"/>
-      <c r="Q1" s="81"/>
-      <c r="R1" s="81"/>
-      <c r="S1" s="81"/>
-      <c r="T1" s="81"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="80">
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="82">
         <f ca="1">V2</f>
         <v>44882</v>
       </c>
-      <c r="W1" s="81"/>
-      <c r="X1" s="81"/>
-      <c r="Y1" s="81"/>
-      <c r="Z1" s="81"/>
-      <c r="AA1" s="81"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="80">
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
+      <c r="AA1" s="83"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="82">
         <f ca="1">AC2</f>
         <v>44889</v>
       </c>
-      <c r="AD1" s="81"/>
-      <c r="AE1" s="81"/>
-      <c r="AF1" s="81"/>
-      <c r="AG1" s="81"/>
-      <c r="AH1" s="81"/>
-      <c r="AI1" s="82"/>
+      <c r="AD1" s="83"/>
+      <c r="AE1" s="83"/>
+      <c r="AF1" s="83"/>
+      <c r="AG1" s="83"/>
+      <c r="AH1" s="83"/>
+      <c r="AI1" s="84"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
       </c>
       <c r="C2" s="60"/>
       <c r="D2" s="60"/>
@@ -3697,28 +3640,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:AI31">
-    <cfRule type="expression" dxfId="11" priority="33">
+    <cfRule type="expression" dxfId="5" priority="33">
       <formula>AND(TODAY()&gt;=H$2,TODAY()&lt;I$2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI2:AI31">
-    <cfRule type="expression" dxfId="10" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="41" stopIfTrue="1">
       <formula>AND(TODAY()&gt;=AI$2,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:AI31">
-    <cfRule type="expression" dxfId="9" priority="27">
+    <cfRule type="expression" dxfId="3" priority="27">
       <formula>AND(task_start&lt;=H$2,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="28" stopIfTrue="1">
       <formula>AND(task_end&gt;=H$2,task_start&lt;I$2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI4:AI31">
-    <cfRule type="expression" dxfId="7" priority="44">
+    <cfRule type="expression" dxfId="1" priority="44">
       <formula>AND(task_start&lt;=AI$2,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=AI$2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="45" stopIfTrue="1">
       <formula>AND(task_end&gt;=AI$2,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3859,12 +3802,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4156,29 +4110,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4205,13 +4159,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Gantt Chart now including software tasks
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{4041CFB6-8B8A-4744-9124-A8F1B5A78BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5E05D61-0122-0C47-85F4-0528842FC30D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25240" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="25245" windowHeight="17505"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <definedName name="task_start" localSheetId="0">ProjectSchedule!$E1</definedName>
     <definedName name="today" localSheetId="0">TODAY()</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -108,21 +107,6 @@
     <t>TASK</t>
   </si>
   <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
   <si>
@@ -275,16 +259,31 @@
   <si>
     <t>Competition time!</t>
   </si>
+  <si>
+    <t>Learn Arduino</t>
+  </si>
+  <si>
+    <t>Block detection software</t>
+  </si>
+  <si>
+    <t>Block sorting software</t>
+  </si>
+  <si>
+    <t>Adding redundancies and updating code</t>
+  </si>
+  <si>
+    <t>Testing feasibility of different means of detection</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="8">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="ddd\,\ dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="d/m/yy;@"/>
     <numFmt numFmtId="168" formatCode="d"/>
@@ -1000,7 +999,7 @@
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="3" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
@@ -1022,9 +1021,9 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1221,9 +1220,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1300,6 +1296,9 @@
     </xf>
     <xf numFmtId="169" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1334,7 +1333,7 @@
     <cellStyle name="Comma [0]" xfId="14" builtinId="6" customBuiltin="1"/>
     <cellStyle name="Currency" xfId="15" builtinId="4" customBuiltin="1"/>
     <cellStyle name="Currency [0]" xfId="16" builtinId="7" customBuiltin="1"/>
-    <cellStyle name="Date" xfId="10" xr:uid="{229918B6-DD13-4F5A-97B9-305F7E002AA3}"/>
+    <cellStyle name="Date" xfId="10"/>
     <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" customBuiltin="1"/>
     <cellStyle name="Good" xfId="18" builtinId="26" customBuiltin="1"/>
@@ -1345,18 +1344,18 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Input" xfId="21" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="24" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Name" xfId="11" xr:uid="{B2D3C1EE-6B41-4801-AAFC-C2274E49E503}"/>
+    <cellStyle name="Name" xfId="11"/>
     <cellStyle name="Neutral" xfId="20" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="27" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="22" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Per cent" xfId="2" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Project Start" xfId="9" xr:uid="{8EB8A09A-C31C-40A3-B2C1-9449520178B8}"/>
-    <cellStyle name="Task" xfId="12" xr:uid="{6391D789-272B-4DD2-9BF3-2CDCF610FA41}"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Project Start" xfId="9"/>
+    <cellStyle name="Task" xfId="12"/>
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="29" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="26" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
+    <cellStyle name="zHiddenText" xfId="3"/>
   </cellStyles>
   <dxfs count="15">
     <dxf>
@@ -1514,7 +1513,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="ToDoList" pivot="0" count="9">
       <tableStyleElement type="wholeTable" dxfId="14"/>
       <tableStyleElement type="headerRow" dxfId="13"/>
       <tableStyleElement type="totalRow" dxfId="12"/>
@@ -1934,214 +1933,214 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V11" sqref="V11"/>
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="40" customWidth="1"/>
-    <col min="2" max="2" width="44.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
-    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="35" width="3.83203125" customWidth="1"/>
-    <col min="40" max="41" width="10.33203125"/>
+    <col min="1" max="1" width="2.7109375" style="40" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="35" width="3.85546875" customWidth="1"/>
+    <col min="40" max="41" width="10.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="81">
+        <v>36</v>
+      </c>
+      <c r="D1" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="80">
         <f ca="1">TODAY()</f>
         <v>44868</v>
       </c>
-      <c r="F1" s="81"/>
-      <c r="H1" s="82">
+      <c r="F1" s="80"/>
+      <c r="H1" s="81">
         <f ca="1">H2</f>
         <v>44868</v>
       </c>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="82">
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="81">
         <f ca="1">O2</f>
         <v>44875</v>
       </c>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="82">
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="81">
         <f ca="1">V2</f>
         <v>44882</v>
       </c>
-      <c r="W1" s="83"/>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
-      <c r="Z1" s="83"/>
-      <c r="AA1" s="83"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="82">
+      <c r="W1" s="82"/>
+      <c r="X1" s="82"/>
+      <c r="Y1" s="82"/>
+      <c r="Z1" s="82"/>
+      <c r="AA1" s="82"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="81">
         <f ca="1">AC2</f>
         <v>44889</v>
       </c>
-      <c r="AD1" s="83"/>
-      <c r="AE1" s="83"/>
-      <c r="AF1" s="83"/>
-      <c r="AG1" s="83"/>
-      <c r="AH1" s="83"/>
-      <c r="AI1" s="84"/>
-    </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD1" s="82"/>
+      <c r="AE1" s="82"/>
+      <c r="AF1" s="82"/>
+      <c r="AG1" s="82"/>
+      <c r="AH1" s="82"/>
+      <c r="AI1" s="83"/>
+    </row>
+    <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="H2" s="77">
+        <v>56</v>
+      </c>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="H2" s="76">
         <f ca="1">Project_Start</f>
         <v>44868</v>
       </c>
-      <c r="I2" s="78">
+      <c r="I2" s="77">
         <f ca="1">H2+1</f>
         <v>44869</v>
       </c>
-      <c r="J2" s="78">
+      <c r="J2" s="77">
         <f t="shared" ref="J2:AI2" ca="1" si="0">I2+1</f>
         <v>44870</v>
       </c>
-      <c r="K2" s="78">
+      <c r="K2" s="77">
         <f t="shared" ca="1" si="0"/>
         <v>44871</v>
       </c>
-      <c r="L2" s="78">
+      <c r="L2" s="77">
         <f t="shared" ca="1" si="0"/>
         <v>44872</v>
       </c>
-      <c r="M2" s="78">
+      <c r="M2" s="77">
         <f t="shared" ca="1" si="0"/>
         <v>44873</v>
       </c>
-      <c r="N2" s="79">
+      <c r="N2" s="78">
         <f t="shared" ca="1" si="0"/>
         <v>44874</v>
       </c>
-      <c r="O2" s="77">
+      <c r="O2" s="76">
         <f ca="1">N2+1</f>
         <v>44875</v>
       </c>
-      <c r="P2" s="78">
+      <c r="P2" s="77">
         <f ca="1">O2+1</f>
         <v>44876</v>
       </c>
-      <c r="Q2" s="78">
+      <c r="Q2" s="77">
         <f t="shared" ca="1" si="0"/>
         <v>44877</v>
       </c>
-      <c r="R2" s="78">
+      <c r="R2" s="77">
         <f ca="1">Q2+1</f>
         <v>44878</v>
       </c>
-      <c r="S2" s="78">
+      <c r="S2" s="77">
         <f t="shared" ca="1" si="0"/>
         <v>44879</v>
       </c>
-      <c r="T2" s="78">
+      <c r="T2" s="77">
         <f t="shared" ca="1" si="0"/>
         <v>44880</v>
       </c>
-      <c r="U2" s="79">
+      <c r="U2" s="78">
         <f t="shared" ca="1" si="0"/>
         <v>44881</v>
       </c>
-      <c r="V2" s="77">
+      <c r="V2" s="76">
         <f ca="1">U2+1</f>
         <v>44882</v>
       </c>
-      <c r="W2" s="78">
+      <c r="W2" s="77">
         <f ca="1">V2+1</f>
         <v>44883</v>
       </c>
-      <c r="X2" s="78">
+      <c r="X2" s="77">
         <f t="shared" ca="1" si="0"/>
         <v>44884</v>
       </c>
-      <c r="Y2" s="78">
+      <c r="Y2" s="77">
         <f t="shared" ca="1" si="0"/>
         <v>44885</v>
       </c>
-      <c r="Z2" s="78">
+      <c r="Z2" s="77">
         <f t="shared" ca="1" si="0"/>
         <v>44886</v>
       </c>
-      <c r="AA2" s="78">
+      <c r="AA2" s="77">
         <f t="shared" ca="1" si="0"/>
         <v>44887</v>
       </c>
-      <c r="AB2" s="79">
+      <c r="AB2" s="78">
         <f t="shared" ca="1" si="0"/>
         <v>44888</v>
       </c>
-      <c r="AC2" s="77">
+      <c r="AC2" s="76">
         <f ca="1">AB2+1</f>
         <v>44889</v>
       </c>
-      <c r="AD2" s="78">
+      <c r="AD2" s="77">
         <f ca="1">AC2+1</f>
         <v>44890</v>
       </c>
-      <c r="AE2" s="78">
+      <c r="AE2" s="77">
         <f t="shared" ca="1" si="0"/>
         <v>44891</v>
       </c>
-      <c r="AF2" s="78">
+      <c r="AF2" s="77">
         <f t="shared" ca="1" si="0"/>
         <v>44892</v>
       </c>
-      <c r="AG2" s="78">
+      <c r="AG2" s="77">
         <f t="shared" ca="1" si="0"/>
         <v>44893</v>
       </c>
-      <c r="AH2" s="78">
+      <c r="AH2" s="77">
         <f t="shared" ca="1" si="0"/>
         <v>44894</v>
       </c>
-      <c r="AI2" s="79">
+      <c r="AI2" s="78">
         <f t="shared" ca="1" si="0"/>
         <v>44895</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
@@ -2149,19 +2148,19 @@
         <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="H3" s="6" t="str">
         <f t="shared" ref="H3" ca="1" si="1">LEFT(TEXT(H2,"ddd"),1)</f>
@@ -2276,7 +2275,7 @@
         <v>W</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="40" t="s">
         <v>3</v>
       </c>
@@ -2315,19 +2314,19 @@
       <c r="AH4" s="27"/>
       <c r="AI4" s="27"/>
     </row>
-    <row r="5" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="41" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D5" s="12"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="63"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="62"/>
       <c r="G5" s="10" t="str">
         <f t="shared" ref="G5:G31" si="3">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
@@ -2361,24 +2360,24 @@
       <c r="AH5" s="27"/>
       <c r="AI5" s="27"/>
     </row>
-    <row r="6" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="41" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D6" s="13">
         <v>0.2</v>
       </c>
-      <c r="E6" s="64">
+      <c r="E6" s="63">
         <f ca="1">Project_Start</f>
         <v>44868</v>
       </c>
-      <c r="F6" s="64">
+      <c r="F6" s="63">
         <f ca="1">E6+3</f>
         <v>44871</v>
       </c>
@@ -2415,21 +2414,21 @@
       <c r="AH6" s="27"/>
       <c r="AI6" s="27"/>
     </row>
-    <row r="7" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="41" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="13">
         <v>0.2</v>
       </c>
-      <c r="E7" s="64">
+      <c r="E7" s="63">
         <v>44868</v>
       </c>
-      <c r="F7" s="64">
+      <c r="F7" s="63">
         <v>44871</v>
       </c>
       <c r="G7" s="10">
@@ -2465,19 +2464,19 @@
       <c r="AH7" s="27"/>
       <c r="AI7" s="27"/>
     </row>
-    <row r="8" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="40"/>
       <c r="B8" s="55" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="13">
         <v>0.2</v>
       </c>
-      <c r="E8" s="64">
+      <c r="E8" s="63">
         <v>44871</v>
       </c>
-      <c r="F8" s="64">
+      <c r="F8" s="63">
         <f>E8+4</f>
         <v>44875</v>
       </c>
@@ -2514,19 +2513,19 @@
       <c r="AH8" s="27"/>
       <c r="AI8" s="27"/>
     </row>
-    <row r="9" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="40"/>
       <c r="B9" s="55" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C9" s="47"/>
       <c r="D9" s="13">
         <v>0</v>
       </c>
-      <c r="E9" s="64">
+      <c r="E9" s="63">
         <v>44871</v>
       </c>
-      <c r="F9" s="64">
+      <c r="F9" s="63">
         <f>E9+5</f>
         <v>44876</v>
       </c>
@@ -2563,20 +2562,20 @@
       <c r="AH9" s="27"/>
       <c r="AI9" s="27"/>
     </row>
-    <row r="10" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="40"/>
       <c r="B10" s="55" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="13">
         <v>0</v>
       </c>
-      <c r="E10" s="64">
+      <c r="E10" s="63">
         <f>E7+1</f>
         <v>44869</v>
       </c>
-      <c r="F10" s="64">
+      <c r="F10" s="63">
         <f>E10+2</f>
         <v>44871</v>
       </c>
@@ -2613,19 +2612,19 @@
       <c r="AH10" s="27"/>
       <c r="AI10" s="27"/>
     </row>
-    <row r="11" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="41" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D11" s="15"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="66"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="65"/>
       <c r="G11" s="10" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2659,19 +2658,19 @@
       <c r="AH11" s="27"/>
       <c r="AI11" s="27"/>
     </row>
-    <row r="12" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="41"/>
       <c r="B12" s="56" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C12" s="49"/>
       <c r="D12" s="16">
         <v>0.2</v>
       </c>
-      <c r="E12" s="67">
+      <c r="E12" s="66">
         <v>44868</v>
       </c>
-      <c r="F12" s="67">
+      <c r="F12" s="66">
         <f>E12+4</f>
         <v>44872</v>
       </c>
@@ -2708,19 +2707,19 @@
       <c r="AH12" s="27"/>
       <c r="AI12" s="27"/>
     </row>
-    <row r="13" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="40"/>
       <c r="B13" s="56" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C13" s="49"/>
       <c r="D13" s="16">
         <v>0.2</v>
       </c>
-      <c r="E13" s="67">
+      <c r="E13" s="66">
         <v>44868</v>
       </c>
-      <c r="F13" s="67">
+      <c r="F13" s="66">
         <f>E13+5</f>
         <v>44873</v>
       </c>
@@ -2757,20 +2756,20 @@
       <c r="AH13" s="27"/>
       <c r="AI13" s="27"/>
     </row>
-    <row r="14" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="40"/>
       <c r="B14" s="56" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C14" s="49"/>
       <c r="D14" s="16">
         <v>0</v>
       </c>
-      <c r="E14" s="67">
+      <c r="E14" s="66">
         <f>F13</f>
         <v>44873</v>
       </c>
-      <c r="F14" s="67">
+      <c r="F14" s="66">
         <v>44874</v>
       </c>
       <c r="G14" s="10">
@@ -2806,20 +2805,20 @@
       <c r="AH14" s="27"/>
       <c r="AI14" s="27"/>
     </row>
-    <row r="15" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="40"/>
       <c r="B15" s="56" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C15" s="49"/>
       <c r="D15" s="16">
         <v>0</v>
       </c>
-      <c r="E15" s="67">
+      <c r="E15" s="66">
         <f>E14</f>
         <v>44873</v>
       </c>
-      <c r="F15" s="67">
+      <c r="F15" s="66">
         <f>E15+2</f>
         <v>44875</v>
       </c>
@@ -2856,19 +2855,19 @@
       <c r="AH15" s="27"/>
       <c r="AI15" s="27"/>
     </row>
-    <row r="16" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="40"/>
       <c r="B16" s="56" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="16">
         <v>0</v>
       </c>
-      <c r="E16" s="67">
+      <c r="E16" s="66">
         <v>44879</v>
       </c>
-      <c r="F16" s="67">
+      <c r="F16" s="66">
         <f>E16+3</f>
         <v>44882</v>
       </c>
@@ -2905,19 +2904,19 @@
       <c r="AH16" s="27"/>
       <c r="AI16" s="27"/>
     </row>
-    <row r="17" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="40"/>
       <c r="B17" s="56" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C17" s="49"/>
       <c r="D17" s="16">
         <v>0</v>
       </c>
-      <c r="E17" s="67">
+      <c r="E17" s="66">
         <v>44879</v>
       </c>
-      <c r="F17" s="67">
+      <c r="F17" s="66">
         <v>44882</v>
       </c>
       <c r="G17" s="10">
@@ -2953,19 +2952,19 @@
       <c r="AH17" s="27"/>
       <c r="AI17" s="27"/>
     </row>
-    <row r="18" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D18" s="18"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="69"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="68"/>
       <c r="G18" s="10" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2999,25 +2998,24 @@
       <c r="AH18" s="27"/>
       <c r="AI18" s="27"/>
     </row>
-    <row r="19" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="40"/>
-      <c r="B19" s="57" t="s">
-        <v>12</v>
+      <c r="B19" s="84" t="s">
+        <v>61</v>
       </c>
       <c r="C19" s="51"/>
       <c r="D19" s="19">
         <v>0</v>
       </c>
-      <c r="E19" s="70">
+      <c r="E19" s="69">
         <v>44868</v>
       </c>
-      <c r="F19" s="70">
-        <f>E19+5</f>
-        <v>44873</v>
+      <c r="F19" s="69">
+        <v>44872</v>
       </c>
       <c r="G19" s="10">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="27"/>
@@ -3048,26 +3046,25 @@
       <c r="AH19" s="27"/>
       <c r="AI19" s="27"/>
     </row>
-    <row r="20" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="40"/>
-      <c r="B20" s="57" t="s">
-        <v>13</v>
+      <c r="B20" s="84" t="s">
+        <v>62</v>
       </c>
       <c r="C20" s="51"/>
       <c r="D20" s="19">
         <v>0</v>
       </c>
-      <c r="E20" s="70">
+      <c r="E20" s="69">
         <f>F19+1</f>
-        <v>44874</v>
-      </c>
-      <c r="F20" s="70">
-        <f>E20+4</f>
-        <v>44878</v>
+        <v>44873</v>
+      </c>
+      <c r="F20" s="69">
+        <v>44879</v>
       </c>
       <c r="G20" s="10">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H20" s="27"/>
       <c r="I20" s="27"/>
@@ -3098,22 +3095,22 @@
       <c r="AH20" s="27"/>
       <c r="AI20" s="27"/>
     </row>
-    <row r="21" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="40"/>
-      <c r="B21" s="57" t="s">
-        <v>14</v>
+      <c r="B21" s="84" t="s">
+        <v>63</v>
       </c>
       <c r="C21" s="51"/>
       <c r="D21" s="19">
         <v>0</v>
       </c>
-      <c r="E21" s="70">
+      <c r="E21" s="69">
         <f>E20+5</f>
-        <v>44879</v>
-      </c>
-      <c r="F21" s="70">
+        <v>44878</v>
+      </c>
+      <c r="F21" s="69">
         <f>E21+5</f>
-        <v>44884</v>
+        <v>44883</v>
       </c>
       <c r="G21" s="10">
         <f t="shared" si="3"/>
@@ -3148,22 +3145,22 @@
       <c r="AH21" s="27"/>
       <c r="AI21" s="27"/>
     </row>
-    <row r="22" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="40"/>
-      <c r="B22" s="57" t="s">
-        <v>15</v>
+      <c r="B22" s="84" t="s">
+        <v>64</v>
       </c>
       <c r="C22" s="51"/>
       <c r="D22" s="19">
         <v>0</v>
       </c>
-      <c r="E22" s="70">
+      <c r="E22" s="69">
         <f>F21+1</f>
-        <v>44885</v>
-      </c>
-      <c r="F22" s="70">
+        <v>44884</v>
+      </c>
+      <c r="F22" s="69">
         <f>E22+4</f>
-        <v>44889</v>
+        <v>44888</v>
       </c>
       <c r="G22" s="10">
         <f t="shared" si="3"/>
@@ -3198,22 +3195,21 @@
       <c r="AH22" s="27"/>
       <c r="AI22" s="27"/>
     </row>
-    <row r="23" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="40"/>
-      <c r="B23" s="57" t="s">
-        <v>16</v>
+      <c r="B23" s="84" t="s">
+        <v>65</v>
       </c>
       <c r="C23" s="51"/>
       <c r="D23" s="19">
         <v>0</v>
       </c>
-      <c r="E23" s="70">
-        <f>E21</f>
-        <v>44879</v>
-      </c>
-      <c r="F23" s="70">
+      <c r="E23" s="69">
+        <v>44871</v>
+      </c>
+      <c r="F23" s="69">
         <f>E23+4</f>
-        <v>44883</v>
+        <v>44875</v>
       </c>
       <c r="G23" s="10">
         <f t="shared" si="3"/>
@@ -3248,19 +3244,19 @@
       <c r="AH23" s="27"/>
       <c r="AI23" s="27"/>
     </row>
-    <row r="24" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C24" s="52" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D24" s="21"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="72"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="71"/>
       <c r="G24" s="10" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3294,17 +3290,17 @@
       <c r="AH24" s="27"/>
       <c r="AI24" s="27"/>
     </row>
-    <row r="25" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="40"/>
-      <c r="B25" s="58" t="s">
-        <v>60</v>
+      <c r="B25" s="57" t="s">
+        <v>55</v>
       </c>
       <c r="C25" s="53"/>
       <c r="D25" s="22"/>
-      <c r="E25" s="73">
+      <c r="E25" s="72">
         <v>44885</v>
       </c>
-      <c r="F25" s="73">
+      <c r="F25" s="72">
         <v>44888</v>
       </c>
       <c r="G25" s="10">
@@ -3340,17 +3336,17 @@
       <c r="AH25" s="27"/>
       <c r="AI25" s="27"/>
     </row>
-    <row r="26" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="40"/>
-      <c r="B26" s="58" t="s">
-        <v>61</v>
+      <c r="B26" s="57" t="s">
+        <v>56</v>
       </c>
       <c r="C26" s="53"/>
       <c r="D26" s="22"/>
-      <c r="E26" s="73">
+      <c r="E26" s="72">
         <v>44888</v>
       </c>
-      <c r="F26" s="73">
+      <c r="F26" s="72">
         <v>44891</v>
       </c>
       <c r="G26" s="10">
@@ -3386,17 +3382,17 @@
       <c r="AH26" s="27"/>
       <c r="AI26" s="27"/>
     </row>
-    <row r="27" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="40"/>
-      <c r="B27" s="58" t="s">
-        <v>62</v>
+      <c r="B27" s="57" t="s">
+        <v>57</v>
       </c>
       <c r="C27" s="53"/>
       <c r="D27" s="22"/>
-      <c r="E27" s="73">
+      <c r="E27" s="72">
         <v>44892</v>
       </c>
-      <c r="F27" s="73">
+      <c r="F27" s="72">
         <v>44893</v>
       </c>
       <c r="G27" s="10">
@@ -3432,17 +3428,17 @@
       <c r="AH27" s="27"/>
       <c r="AI27" s="27"/>
     </row>
-    <row r="28" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="40"/>
-      <c r="B28" s="58" t="s">
-        <v>63</v>
+      <c r="B28" s="57" t="s">
+        <v>58</v>
       </c>
       <c r="C28" s="53"/>
       <c r="D28" s="22"/>
-      <c r="E28" s="73">
+      <c r="E28" s="72">
         <v>44894</v>
       </c>
-      <c r="F28" s="73">
+      <c r="F28" s="72">
         <v>44895</v>
       </c>
       <c r="G28" s="10">
@@ -3478,17 +3474,17 @@
       <c r="AH28" s="27"/>
       <c r="AI28" s="27"/>
     </row>
-    <row r="29" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="40"/>
-      <c r="B29" s="58" t="s">
-        <v>65</v>
+      <c r="B29" s="57" t="s">
+        <v>60</v>
       </c>
       <c r="C29" s="53"/>
       <c r="D29" s="22"/>
-      <c r="E29" s="73">
+      <c r="E29" s="72">
         <v>44894</v>
       </c>
-      <c r="F29" s="73">
+      <c r="F29" s="72">
         <v>44895</v>
       </c>
       <c r="G29" s="10">
@@ -3524,15 +3520,15 @@
       <c r="AH29" s="27"/>
       <c r="AI29" s="27"/>
     </row>
-    <row r="30" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="59"/>
+      <c r="B30" s="58"/>
       <c r="C30" s="54"/>
       <c r="D30" s="9"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="73"/>
       <c r="G30" s="10" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3566,17 +3562,17 @@
       <c r="AH30" s="27"/>
       <c r="AI30" s="27"/>
     </row>
-    <row r="31" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="41" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C31" s="24"/>
       <c r="D31" s="25"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="76"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="75"/>
       <c r="G31" s="26" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3610,11 +3606,11 @@
       <c r="AH31" s="29"/>
       <c r="AI31" s="29"/>
     </row>
-    <row r="33" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="7"/>
       <c r="F33" s="42"/>
     </row>
-    <row r="34" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="8"/>
     </row>
   </sheetData>
@@ -3672,7 +3668,7 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="F15 F20:F21 E21" formula="1"/>
+    <ignoredError sqref="F15 F21 E21" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -3699,101 +3695,101 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="87.1640625" style="30" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="87.140625" style="30" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:2" s="32" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2" s="31"/>
     </row>
-    <row r="3" spans="1:2" s="36" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="61" t="s">
-        <v>26</v>
+    <row r="3" spans="1:2" s="36" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>21</v>
       </c>
       <c r="B3" s="37"/>
     </row>
-    <row r="4" spans="1:2" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="33" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="34" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="35" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="30" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="33" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A8" s="34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.2">
+      <c r="A9" s="35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="30" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="33" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A11" s="34" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="30" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="39" t="s">
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="35" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
+    <row r="13" spans="1:2" s="30" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="48" x14ac:dyDescent="0.2">
-      <c r="A9" s="35" t="s">
+    <row r="14" spans="1:2" s="33" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A14" s="34" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="30" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A11" s="34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="30" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A14" s="34" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.2">
       <c r="A16" s="35" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="A2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="A13" r:id="rId1"/>
+    <hyperlink ref="A10" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -3802,23 +3798,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4110,29 +4095,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4159,9 +4144,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>